<commit_message>
fix validation while uploading siswa using excel
</commit_message>
<xml_diff>
--- a/public/excel/single/bts.xlsx
+++ b/public/excel/single/bts.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>d_kelas</t>
   </si>
@@ -46,31 +46,31 @@
     <t>nama</t>
   </si>
   <si>
-    <t>no system is safe</t>
-  </si>
-  <si>
     <t>Si_A.jpg</t>
   </si>
   <si>
     <t>Si_B.jpg</t>
   </si>
   <si>
-    <t>ah boong kali lu A</t>
-  </si>
-  <si>
-    <t>TET</t>
-  </si>
-  <si>
     <t>nis</t>
   </si>
   <si>
-    <t>Martha</t>
-  </si>
-  <si>
-    <t>Koko</t>
-  </si>
-  <si>
     <t>TKJ</t>
+  </si>
+  <si>
+    <t>not error</t>
+  </si>
+  <si>
+    <t>tei</t>
+  </si>
+  <si>
+    <t>Si_C.jpg</t>
+  </si>
+  <si>
+    <t>si_D.jpg</t>
+  </si>
+  <si>
+    <t>ah masa</t>
   </si>
 </sst>
 </file>
@@ -422,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -438,7 +438,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -458,19 +458,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>192010235</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -478,22 +478,62 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>192010036</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix validation while uploading siswa using excel 2
</commit_message>
<xml_diff>
--- a/public/excel/single/bts.xlsx
+++ b/public/excel/single/bts.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>d_kelas</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>ah masa</t>
+  </si>
+  <si>
+    <t>tbsm</t>
   </si>
 </sst>
 </file>
@@ -425,7 +428,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -510,7 +513,7 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -533,7 +536,7 @@
         <v>8</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upload class ak2 students
</commit_message>
<xml_diff>
--- a/public/excel/single/bts.xlsx
+++ b/public/excel/single/bts.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafly/Documents/BTS/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831978C3-6628-2644-A485-EE803A539D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="495" windowWidth="19440" windowHeight="12240"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16220" xr2:uid="{75501D65-3965-EE43-811D-9DB898D7CB65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="106">
   <si>
     <t>d_kelas</t>
   </si>
@@ -46,47 +52,333 @@
     <t>nama</t>
   </si>
   <si>
-    <t>Si_A.jpg</t>
-  </si>
-  <si>
-    <t>Si_B.jpg</t>
-  </si>
-  <si>
     <t>nis</t>
   </si>
   <si>
-    <t>TKJ</t>
-  </si>
-  <si>
-    <t>not error</t>
-  </si>
-  <si>
-    <t>tei</t>
-  </si>
-  <si>
-    <t>Si_C.jpg</t>
-  </si>
-  <si>
-    <t>si_D.jpg</t>
-  </si>
-  <si>
-    <t>ah masa</t>
-  </si>
-  <si>
-    <t>tbsm</t>
+    <t>Afrilia Herawati</t>
+  </si>
+  <si>
+    <t>Alifah Wulandari</t>
+  </si>
+  <si>
+    <t>Anggelita Febriyanti</t>
+  </si>
+  <si>
+    <t>Ariel Faqih Muzhaffar</t>
+  </si>
+  <si>
+    <t>Ayestania Hedita</t>
+  </si>
+  <si>
+    <t>Azalia Dalawir</t>
+  </si>
+  <si>
+    <t>Choirunnisa</t>
+  </si>
+  <si>
+    <t>Diah Ayu Frimanda</t>
+  </si>
+  <si>
+    <t>Dini Al-Adawiah</t>
+  </si>
+  <si>
+    <t>Eliniawati</t>
+  </si>
+  <si>
+    <t>Firda Arlina Hudoyo</t>
+  </si>
+  <si>
+    <t>Ghina Nabilah Fauziyyah</t>
+  </si>
+  <si>
+    <t>Iin Indah Sari</t>
+  </si>
+  <si>
+    <t>Lira Aulia Nurahman</t>
+  </si>
+  <si>
+    <t>Mariah</t>
+  </si>
+  <si>
+    <t>Mirna Sartika</t>
+  </si>
+  <si>
+    <t>Munjiah Asliani</t>
+  </si>
+  <si>
+    <t>Namira Putri Karpali</t>
+  </si>
+  <si>
+    <t>Nilam Ayu Prasetya</t>
+  </si>
+  <si>
+    <t>Nisa Pebiyanti</t>
+  </si>
+  <si>
+    <t>Noklina</t>
+  </si>
+  <si>
+    <t>Putri Indiana Sari</t>
+  </si>
+  <si>
+    <t>Qurratu A'ini</t>
+  </si>
+  <si>
+    <t>Rizka Habibah</t>
+  </si>
+  <si>
+    <t>Sabrina Karimah Putri</t>
+  </si>
+  <si>
+    <t>Selly Septinur Rohmah</t>
+  </si>
+  <si>
+    <t>Selpia</t>
+  </si>
+  <si>
+    <t>Siti Fatimah</t>
+  </si>
+  <si>
+    <t>Siti Munaroh</t>
+  </si>
+  <si>
+    <t>Suryani Tirta Lestari</t>
+  </si>
+  <si>
+    <t>Syarifah</t>
+  </si>
+  <si>
+    <t>Trista Ananda</t>
+  </si>
+  <si>
+    <t>Yunitsa Rakhmawati</t>
+  </si>
+  <si>
+    <t>afrilia_herawati.jpg</t>
+  </si>
+  <si>
+    <t>alifah_wulandari.jpg</t>
+  </si>
+  <si>
+    <t>anggelita_febriyanti.jpg</t>
+  </si>
+  <si>
+    <t>ariel_faqih_muzhaffar.jpg</t>
+  </si>
+  <si>
+    <t>ayestania_hedita.jpg</t>
+  </si>
+  <si>
+    <t>azalia_dalawir.jpg</t>
+  </si>
+  <si>
+    <t>choirunnisa.jpg</t>
+  </si>
+  <si>
+    <t>diah_ayu_frismanda.jpg</t>
+  </si>
+  <si>
+    <t>dini_al-adawiah.jpg</t>
+  </si>
+  <si>
+    <t>eliniawati.jpg</t>
+  </si>
+  <si>
+    <t>firda_arlina_hudoyo.jpg</t>
+  </si>
+  <si>
+    <t>ghina_nabilah_fauziyyah.jpg</t>
+  </si>
+  <si>
+    <t>iin_indah_sari.JPG</t>
+  </si>
+  <si>
+    <t>lira_aulia_nurahman.jpg</t>
+  </si>
+  <si>
+    <t>mariah.jpg</t>
+  </si>
+  <si>
+    <t>mirna_sartika.jpg</t>
+  </si>
+  <si>
+    <t>munjiah_asliani.jpg</t>
+  </si>
+  <si>
+    <t>namira_putri_karpali.JPG</t>
+  </si>
+  <si>
+    <t>nilam_ayu_prasetya.JPG</t>
+  </si>
+  <si>
+    <t>nisa_pebiyanti.jpg</t>
+  </si>
+  <si>
+    <t>noklina.jpg</t>
+  </si>
+  <si>
+    <t>putri_indiana_sari.jpeg</t>
+  </si>
+  <si>
+    <t>qurratu_a'ini.jpg</t>
+  </si>
+  <si>
+    <t>rizka_habibah.JPG</t>
+  </si>
+  <si>
+    <t>sabrina_karimah_putri.jpg</t>
+  </si>
+  <si>
+    <t>selly_septinur_romah.jpg</t>
+  </si>
+  <si>
+    <t>selpia.jpg</t>
+  </si>
+  <si>
+    <t>siti_fatimah.jpeg</t>
+  </si>
+  <si>
+    <t>siti_munaroh.jpg</t>
+  </si>
+  <si>
+    <t>suryani_tirta_lestari.jpeg</t>
+  </si>
+  <si>
+    <t>syarifah.JPG</t>
+  </si>
+  <si>
+    <t>trista_ananda.jpg</t>
+  </si>
+  <si>
+    <t>yunitsa_rakhmawati.JPG</t>
+  </si>
+  <si>
+    <t>Trust your journey even if the road seems a little rough at times, you'll get there.</t>
+  </si>
+  <si>
+    <t>Living only once is wrong. We live every day and die once.</t>
+  </si>
+  <si>
+    <t>Hidup sesuai kemampuan, bukan kemauan.</t>
+  </si>
+  <si>
+    <t>Kita adalah pernah, bukan punah, bukan menyerah, hanya sudah.</t>
+  </si>
+  <si>
+    <t>You were born to be real, not be perfect.</t>
+  </si>
+  <si>
+    <t>From zero to hero, from nothing to something.</t>
+  </si>
+  <si>
+    <t>Jangan beri tahu orang-orang tentang rencanamu. Tapi, tunjukkan pada mereka hasilmu.</t>
+  </si>
+  <si>
+    <t>Study now, be proud later.</t>
+  </si>
+  <si>
+    <t>Every day, Take a Step to Grow up.</t>
+  </si>
+  <si>
+    <t>Be yourself because no one wants to be you.</t>
+  </si>
+  <si>
+    <t>Mau + tapi = konflik</t>
+  </si>
+  <si>
+    <t>Hardwork will never betray you.</t>
+  </si>
+  <si>
+    <t>Waktu tidak dapat diputar, dijilat, apalagi dicelupin.</t>
+  </si>
+  <si>
+    <t>People who laugh too hard and coughing are the people who, minum too much teajus.</t>
+  </si>
+  <si>
+    <t>Don't just dream but make it happen.</t>
+  </si>
+  <si>
+    <t>Loving yourself isn't vanity, it's sanity.</t>
+  </si>
+  <si>
+    <t>Believe that everything in your life is God's beautiful plan for you.</t>
+  </si>
+  <si>
+    <t>Sich selbst zu lieben ist keine eitelkeit, sondern vernunft.</t>
+  </si>
+  <si>
+    <t>Perjuangan merupakan tanda perjalananmu menuju sukses.</t>
+  </si>
+  <si>
+    <t>i'm only smiling because this is all over.</t>
+  </si>
+  <si>
+    <t>Jangan bandingkan proses mu dengan orang lain karna tidak semua bunga mekar secara bersamaan.</t>
+  </si>
+  <si>
+    <t>Hargai kedua orang tuamu, mereka berhasil lulus sekolah tanpa bantuan google.</t>
+  </si>
+  <si>
+    <t>Apapun yang terjadi, teruslah bernafas.</t>
+  </si>
+  <si>
+    <t>Don’t be afraid to give up the good for the great.</t>
+  </si>
+  <si>
+    <t>Human, half of water, half of mager.</t>
+  </si>
+  <si>
+    <t>Do something today that your future self will thank you for.</t>
+  </si>
+  <si>
+    <t>Life will always guide you to what's best for you.</t>
+  </si>
+  <si>
+    <t>Jangan membenci mereka yang ingin menjatuhkanmu, karena merekalah yang buatmu semakin kuat.</t>
+  </si>
+  <si>
+    <t>Motivasi tanpa aksi adalah halusinasi.</t>
+  </si>
+  <si>
+    <t>The happiness we create, don't expect it from others because it will hurt.</t>
+  </si>
+  <si>
+    <t>Kita dilahirkan untuk menjadi nyata bukan sempurna.</t>
+  </si>
+  <si>
+    <t>Ikan hiu makan tomat, Alhamdulillah tamat.</t>
+  </si>
+  <si>
+    <t>Kejarlah akhirat maka dunia akan mengikutimu.</t>
+  </si>
+  <si>
+    <t>AK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -97,7 +389,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -105,12 +397,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -171,7 +504,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -223,7 +556,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -417,31 +750,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F10766E-6AEC-7C4B-9CE3-FD2B503812DD}">
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="15.875" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
-    <col min="4" max="4" width="23.625" customWidth="1"/>
+    <col min="4" max="4" width="66" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -459,84 +792,664 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>192010642</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>192010643</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>192010644</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>192010645</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>192010646</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>192010647</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>192010648</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>192010650</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>192010651</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
+      <c r="C10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>192010652</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>192010653</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>192010654</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" t="s">
+        <v>105</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>192010655</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>192010657</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" t="s">
+        <v>105</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>192010658</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>192010659</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>192010660</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>192010661</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>192010662</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" t="s">
+        <v>105</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>192010663</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>192010664</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <v>192010665</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>192010666</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>192010667</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>192010668</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>192010669</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>192010670</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>192010671</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" t="s">
+        <v>105</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>192010672</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>192010673</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E31" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>192010674</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>192010675</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" t="s">
+        <v>105</v>
+      </c>
+      <c r="F33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>192010676</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F34">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>